<commit_message>
working script w/o formatting
</commit_message>
<xml_diff>
--- a/mice_records/histology.xlsx
+++ b/mice_records/histology.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Mouse Nr.</t>
   </si>
@@ -62,14 +62,42 @@
   </si>
   <si>
     <t>AV678</t>
+  </si>
+  <si>
+    <t>AVI999</t>
+  </si>
+  <si>
+    <t>av567</t>
+  </si>
+  <si>
+    <t>AV544</t>
+  </si>
+  <si>
+    <t>wt/wt</t>
+  </si>
+  <si>
+    <t>AV666</t>
+  </si>
+  <si>
+    <t>AV777</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>AV212</t>
+  </si>
+  <si>
+    <t>AV567</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+  <numFmts count="2">
+    <numFmt formatCode="yyyy\-mm\-dd" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="165"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -80,12 +108,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,10 +134,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -379,15 +415,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="10.7109375"/>
+    <col customWidth="1" max="6" min="6" style="3" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -406,7 +443,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -426,7 +463,7 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -446,7 +483,7 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -466,7 +503,7 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -486,7 +523,7 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -506,7 +543,7 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -526,7 +563,187 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>43014</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>43014</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>43014</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>43014</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>43014</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>43014</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>43014</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>43014</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>43014</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>